<commit_message>
create title and moderator updated
</commit_message>
<xml_diff>
--- a/yii2/web/runtime/export/Titles.xlsx
+++ b/yii2/web/runtime/export/Titles.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Worksheet'!$A$1:$O$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Worksheet'!$A$1:$R$8</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
   <si>
     <t>#</t>
   </si>
@@ -46,6 +46,9 @@
     <t>Co Supervisor</t>
   </si>
   <si>
+    <t>Moderator</t>
+  </si>
+  <si>
     <t>Departments</t>
   </si>
   <si>
@@ -55,10 +58,16 @@
     <t>Equipment Required</t>
   </si>
   <si>
+    <t>Special Requirements</t>
+  </si>
+  <si>
+    <t>Industrial Links</t>
+  </si>
+  <si>
+    <t>Community Projects</t>
+  </si>
+  <si>
     <t>Suitable For Course</t>
-  </si>
-  <si>
-    <t>Moderator</t>
   </si>
   <si>
     <t>Student ID</t>
@@ -128,6 +137,9 @@
     <t>Hoo Mei Hao</t>
   </si>
   <si>
+    <t>Lim Khong Leng</t>
+  </si>
+  <si>
     <t>he purpose of the system is to allow users to plan and book fully customized tour packages according to
 user&amp;#039;s requirement such as budget, destination, number of days of visitation etc, in a tour and travel agency.
 Scope: countries in Southeast Asia
@@ -178,6 +190,27 @@
 - item record
 - item search
 - appreciation/ depreciation calculation of items</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>January 2018</t>
+  </si>
+  <si>
+    <t>testing1</t>
+  </si>
+  <si>
+    <t>testing2</t>
+  </si>
+  <si>
+    <t>testing3</t>
+  </si>
+  <si>
+    <t>testing4</t>
+  </si>
+  <si>
+    <t>testing5</t>
   </si>
 </sst>
 </file>
@@ -538,7 +571,7 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -556,15 +589,18 @@
     <col min="7" max="7" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="18.709717" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="68.269043" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="218.0896" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="38.847656" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="23.422852" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="68.269043" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="218.0896" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="38.847656" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="19.995117" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="22.280273" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="23.422852" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="12.854004" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,8 +646,17 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1</v>
       </c>
@@ -619,46 +664,49 @@
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2">
+        <v>26</v>
+      </c>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2">
         <v>1406354</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>2</v>
       </c>
@@ -666,46 +714,49 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>3</v>
       </c>
@@ -713,46 +764,49 @@
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="M4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4">
+        <v>38</v>
+      </c>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4">
         <v>1406123</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>4</v>
       </c>
@@ -760,46 +814,49 @@
         <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K5" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="M5" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>5</v>
       </c>
@@ -807,46 +864,49 @@
         <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="M6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" t="s">
-        <v>20</v>
+        <v>46</v>
+      </c>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6" t="s">
+        <v>39</v>
+      </c>
+      <c r="R6" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>6</v>
       </c>
@@ -854,46 +914,49 @@
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" t="s">
         <v>32</v>
       </c>
-      <c r="I7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" t="s">
-        <v>20</v>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7" t="s">
+        <v>43</v>
+      </c>
+      <c r="R7" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>7</v>
       </c>
@@ -901,48 +964,107 @@
         <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" t="s">
         <v>32</v>
       </c>
-      <c r="J8" t="s">
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8" t="s">
+        <v>39</v>
+      </c>
+      <c r="R8">
+        <v>1304607</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
         <v>21</v>
       </c>
-      <c r="K8" t="s">
-        <v>44</v>
-      </c>
-      <c r="L8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" t="s">
-        <v>20</v>
-      </c>
-      <c r="O8">
-        <v>1304607</v>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" t="s">
+        <v>53</v>
+      </c>
+      <c r="O9" t="s">
+        <v>54</v>
+      </c>
+      <c r="P9" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R9" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <autoFilter ref="A1:O7"/>
+  <autoFilter ref="A1:R8"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>

</xml_diff>